<commit_message>
Finalizada toda la parte de código de ambas entregas, a escepción de algunos retoques.
</commit_message>
<xml_diff>
--- a/tarea1/outputs/df1.xlsx
+++ b/tarea1/outputs/df1.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E251"/>
+  <dimension ref="A1:F251"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -383,6 +383,11 @@
           <t>c</t>
         </is>
       </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>p_value</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2">
@@ -400,6 +405,9 @@
       <c r="E2">
         <v>-2.006013449399846</v>
       </c>
+      <c r="F2">
+        <v>0.8118811881188119</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3">
@@ -417,6 +425,9 @@
       <c r="E3">
         <v>0.8018226531746249</v>
       </c>
+      <c r="F3">
+        <v>0.06930693069306931</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4">
@@ -434,6 +445,9 @@
       <c r="E4">
         <v>0.9848321893960296</v>
       </c>
+      <c r="F4">
+        <v>0.495049504950495</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5">
@@ -451,6 +465,9 @@
       <c r="E5">
         <v>0.6936201219244138</v>
       </c>
+      <c r="F5">
+        <v>0.9207920792079208</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6">
@@ -468,6 +485,9 @@
       <c r="E6">
         <v>0.5353031032701842</v>
       </c>
+      <c r="F6">
+        <v>0.3663366336633663</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7">
@@ -485,6 +505,9 @@
       <c r="E7">
         <v>-1.168284601062797</v>
       </c>
+      <c r="F7">
+        <v>0.8613861386138614</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8">
@@ -502,6 +525,9 @@
       <c r="E8">
         <v>0.6095258652830369</v>
       </c>
+      <c r="F8">
+        <v>0.3168316831683168</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9">
@@ -519,6 +545,9 @@
       <c r="E9">
         <v>-0.1743103125822338</v>
       </c>
+      <c r="F9">
+        <v>0.2574257425742574</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10">
@@ -536,6 +565,9 @@
       <c r="E10">
         <v>-1.12255569076464</v>
       </c>
+      <c r="F10">
+        <v>0.2871287128712871</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11">
@@ -553,6 +585,9 @@
       <c r="E11">
         <v>-0.3580830483194222</v>
       </c>
+      <c r="F11">
+        <v>0.1683168316831683</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12">
@@ -570,6 +605,9 @@
       <c r="E12">
         <v>-0.8430758469389866</v>
       </c>
+      <c r="F12">
+        <v>0.5841584158415841</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13">
@@ -587,6 +625,9 @@
       <c r="E13">
         <v>1.778375091573751</v>
       </c>
+      <c r="F13">
+        <v>0.2475247524752475</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14">
@@ -604,6 +645,9 @@
       <c r="E14">
         <v>-0.9042542779078486</v>
       </c>
+      <c r="F14">
+        <v>0.7326732673267327</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15">
@@ -621,6 +665,9 @@
       <c r="E15">
         <v>-0.7164908091911453</v>
       </c>
+      <c r="F15">
+        <v>0.198019801980198</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16">
@@ -638,6 +685,9 @@
       <c r="E16">
         <v>1.004304040120748</v>
       </c>
+      <c r="F16">
+        <v>0.693069306930693</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17">
@@ -655,6 +705,9 @@
       <c r="E17">
         <v>-0.9604515170113658</v>
       </c>
+      <c r="F17">
+        <v>0.3861386138613861</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18">
@@ -672,6 +725,9 @@
       <c r="E18">
         <v>-0.7245236812540585</v>
       </c>
+      <c r="F18">
+        <v>0.3267326732673267</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19">
@@ -689,6 +745,9 @@
       <c r="E19">
         <v>-0.7398515542802867</v>
       </c>
+      <c r="F19">
+        <v>0.7227722772277227</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20">
@@ -706,6 +765,9 @@
       <c r="E20">
         <v>-0.9608935484812289</v>
       </c>
+      <c r="F20">
+        <v>0.8316831683168316</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21">
@@ -723,6 +785,9 @@
       <c r="E21">
         <v>-1.417114241346833</v>
       </c>
+      <c r="F21">
+        <v>0.4752475247524752</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22">
@@ -740,6 +805,9 @@
       <c r="E22">
         <v>-0.05396045121472332</v>
       </c>
+      <c r="F22">
+        <v>0.7920792079207921</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23">
@@ -757,6 +825,9 @@
       <c r="E23">
         <v>-0.6583575120627196</v>
       </c>
+      <c r="F23">
+        <v>0.4554455445544555</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24">
@@ -774,6 +845,9 @@
       <c r="E24">
         <v>-0.7303222176274772</v>
       </c>
+      <c r="F24">
+        <v>0.1287128712871287</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25">
@@ -791,6 +865,9 @@
       <c r="E25">
         <v>0.2387976267556151</v>
       </c>
+      <c r="F25">
+        <v>0.2772277227722773</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26">
@@ -808,6 +885,9 @@
       <c r="E26">
         <v>-0.2055194801145111</v>
       </c>
+      <c r="F26">
+        <v>0.2772277227722773</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27">
@@ -825,6 +905,9 @@
       <c r="E27">
         <v>-0.2954469421767925</v>
       </c>
+      <c r="F27">
+        <v>0.09900990099009901</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28">
@@ -842,6 +925,9 @@
       <c r="E28">
         <v>-1.326998905082623</v>
       </c>
+      <c r="F28">
+        <v>0.405940594059406</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29">
@@ -859,6 +945,9 @@
       <c r="E29">
         <v>0.8527203959071942</v>
       </c>
+      <c r="F29">
+        <v>0.5742574257425742</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30">
@@ -876,6 +965,9 @@
       <c r="E30">
         <v>0.857956927271549</v>
       </c>
+      <c r="F30">
+        <v>0.8217821782178217</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31">
@@ -893,6 +985,9 @@
       <c r="E31">
         <v>0.5537276090201529</v>
       </c>
+      <c r="F31">
+        <v>0.0297029702970297</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32">
@@ -910,6 +1005,9 @@
       <c r="E32">
         <v>1.039905297648771</v>
       </c>
+      <c r="F32">
+        <v>0.3069306930693069</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33">
@@ -927,6 +1025,9 @@
       <c r="E33">
         <v>0.1551390928376677</v>
       </c>
+      <c r="F33">
+        <v>0.7722772277227723</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34">
@@ -944,6 +1045,9 @@
       <c r="E34">
         <v>-0.7348483290418534</v>
       </c>
+      <c r="F34">
+        <v>0.1683168316831683</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35">
@@ -961,6 +1065,9 @@
       <c r="E35">
         <v>-0.4913061668969543</v>
       </c>
+      <c r="F35">
+        <v>0.1485148514851485</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36">
@@ -978,6 +1085,9 @@
       <c r="E36">
         <v>1.334550279293454</v>
       </c>
+      <c r="F36">
+        <v>0.7623762376237624</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37">
@@ -995,6 +1105,9 @@
       <c r="E37">
         <v>0.739665373578005</v>
       </c>
+      <c r="F37">
+        <v>0.5544554455445545</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38">
@@ -1012,6 +1125,9 @@
       <c r="E38">
         <v>0.1948428258297443</v>
       </c>
+      <c r="F38">
+        <v>0.5247524752475248</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39">
@@ -1029,6 +1145,9 @@
       <c r="E39">
         <v>0.5824130538827875</v>
       </c>
+      <c r="F39">
+        <v>0.8712871287128713</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40">
@@ -1046,6 +1165,9 @@
       <c r="E40">
         <v>0.3521114579554275</v>
       </c>
+      <c r="F40">
+        <v>0.8910891089108911</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41">
@@ -1063,6 +1185,9 @@
       <c r="E41">
         <v>-0.865711085016065</v>
       </c>
+      <c r="F41">
+        <v>0.693069306930693</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42">
@@ -1080,6 +1205,9 @@
       <c r="E42">
         <v>0.5633509002016699</v>
       </c>
+      <c r="F42">
+        <v>0.8118811881188119</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43">
@@ -1097,6 +1225,9 @@
       <c r="E43">
         <v>-0.4073545063380271</v>
       </c>
+      <c r="F43">
+        <v>0.3069306930693069</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44">
@@ -1114,6 +1245,9 @@
       <c r="E44">
         <v>0.4624921550986888</v>
       </c>
+      <c r="F44">
+        <v>0.1089108910891089</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45">
@@ -1131,6 +1265,9 @@
       <c r="E45">
         <v>0.7939331818384578</v>
       </c>
+      <c r="F45">
+        <v>0.0891089108910891</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46">
@@ -1148,6 +1285,9 @@
       <c r="E46">
         <v>-0.4567644772837369</v>
       </c>
+      <c r="F46">
+        <v>0.7227722772277227</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47">
@@ -1165,6 +1305,9 @@
       <c r="E47">
         <v>-0.5392287102830121</v>
       </c>
+      <c r="F47">
+        <v>0.3366336633663367</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48">
@@ -1182,6 +1325,9 @@
       <c r="E48">
         <v>0.5294240841115584</v>
       </c>
+      <c r="F48">
+        <v>0.7920792079207921</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49">
@@ -1199,6 +1345,9 @@
       <c r="E49">
         <v>-0.5793341211377886</v>
       </c>
+      <c r="F49">
+        <v>0.0198019801980198</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50">
@@ -1216,6 +1365,9 @@
       <c r="E50">
         <v>0.9108954886633501</v>
       </c>
+      <c r="F50">
+        <v>0.5247524752475248</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51">
@@ -1233,6 +1385,9 @@
       <c r="E51">
         <v>-1.042951472909198</v>
       </c>
+      <c r="F51">
+        <v>0.2277227722772277</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52">
@@ -1250,6 +1405,9 @@
       <c r="E52">
         <v>0.757068543906641</v>
       </c>
+      <c r="F52">
+        <v>1</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53">
@@ -1267,6 +1425,9 @@
       <c r="E53">
         <v>0.426419311582469</v>
       </c>
+      <c r="F53">
+        <v>0.5148514851485149</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54">
@@ -1284,6 +1445,9 @@
       <c r="E54">
         <v>0.4488320943474635</v>
       </c>
+      <c r="F54">
+        <v>0.1485148514851485</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55">
@@ -1301,6 +1465,9 @@
       <c r="E55">
         <v>-0.1517082916659516</v>
       </c>
+      <c r="F55">
+        <v>0.2871287128712871</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56">
@@ -1318,6 +1485,9 @@
       <c r="E56">
         <v>0.6668854094461582</v>
       </c>
+      <c r="F56">
+        <v>0.07920792079207921</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57">
@@ -1335,6 +1505,9 @@
       <c r="E57">
         <v>0.7906376164182564</v>
       </c>
+      <c r="F57">
+        <v>0.5643564356435643</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58">
@@ -1352,6 +1525,9 @@
       <c r="E58">
         <v>1.372770551964358</v>
       </c>
+      <c r="F58">
+        <v>0.07920792079207921</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59">
@@ -1369,6 +1545,9 @@
       <c r="E59">
         <v>-1.071857223356334</v>
       </c>
+      <c r="F59">
+        <v>0.5346534653465347</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60">
@@ -1386,6 +1565,9 @@
       <c r="E60">
         <v>-1.059207604491693</v>
       </c>
+      <c r="F60">
+        <v>0.7524752475247525</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61">
@@ -1403,6 +1585,9 @@
       <c r="E61">
         <v>0.6885812699918666</v>
       </c>
+      <c r="F61">
+        <v>0.4455445544554456</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62">
@@ -1420,6 +1605,9 @@
       <c r="E62">
         <v>-0.6479827451599539</v>
       </c>
+      <c r="F62">
+        <v>0.900990099009901</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63">
@@ -1437,6 +1625,9 @@
       <c r="E63">
         <v>-0.7618860460962307</v>
       </c>
+      <c r="F63">
+        <v>0.1881188118811881</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64">
@@ -1454,6 +1645,9 @@
       <c r="E64">
         <v>1.974001836174367</v>
       </c>
+      <c r="F64">
+        <v>0.6435643564356436</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65">
@@ -1471,6 +1665,9 @@
       <c r="E65">
         <v>-1.282068515543343</v>
       </c>
+      <c r="F65">
+        <v>0.1188118811881188</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66">
@@ -1488,6 +1685,9 @@
       <c r="E66">
         <v>0.8887206049484936</v>
       </c>
+      <c r="F66">
+        <v>0.7722772277227723</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67">
@@ -1505,6 +1705,9 @@
       <c r="E67">
         <v>-0.6043529899989203</v>
       </c>
+      <c r="F67">
+        <v>0.0297029702970297</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68">
@@ -1522,6 +1725,9 @@
       <c r="E68">
         <v>-0.902489978139456</v>
       </c>
+      <c r="F68">
+        <v>0.7326732673267327</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69">
@@ -1539,6 +1745,9 @@
       <c r="E69">
         <v>0.5630616376741386</v>
       </c>
+      <c r="F69">
+        <v>0.2673267326732673</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70">
@@ -1556,6 +1765,9 @@
       <c r="E70">
         <v>1.400211747820273</v>
       </c>
+      <c r="F70">
+        <v>0.04950495049504951</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71">
@@ -1573,6 +1785,9 @@
       <c r="E71">
         <v>1.788120278240737</v>
       </c>
+      <c r="F71">
+        <v>0.3960396039603961</v>
+      </c>
     </row>
     <row r="72">
       <c r="A72">
@@ -1590,6 +1805,9 @@
       <c r="E72">
         <v>0.2624512929875739</v>
       </c>
+      <c r="F72">
+        <v>0.3069306930693069</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73">
@@ -1607,6 +1825,9 @@
       <c r="E73">
         <v>1.310831266126302</v>
       </c>
+      <c r="F73">
+        <v>0.5643564356435643</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74">
@@ -1624,6 +1845,9 @@
       <c r="E74">
         <v>-0.9356542646568849</v>
       </c>
+      <c r="F74">
+        <v>0.7524752475247525</v>
+      </c>
     </row>
     <row r="75">
       <c r="A75">
@@ -1641,6 +1865,9 @@
       <c r="E75">
         <v>-0.3142438366636682</v>
       </c>
+      <c r="F75">
+        <v>0.1485148514851485</v>
+      </c>
     </row>
     <row r="76">
       <c r="A76">
@@ -1658,6 +1885,9 @@
       <c r="E76">
         <v>0.6327709756134023</v>
       </c>
+      <c r="F76">
+        <v>0.504950495049505</v>
+      </c>
     </row>
     <row r="77">
       <c r="A77">
@@ -1675,6 +1905,9 @@
       <c r="E77">
         <v>1.216240854253797</v>
       </c>
+      <c r="F77">
+        <v>0.2475247524752475</v>
+      </c>
     </row>
     <row r="78">
       <c r="A78">
@@ -1692,6 +1925,9 @@
       <c r="E78">
         <v>-1.023174505312072</v>
       </c>
+      <c r="F78">
+        <v>0.2079207920792079</v>
+      </c>
     </row>
     <row r="79">
       <c r="A79">
@@ -1709,6 +1945,9 @@
       <c r="E79">
         <v>-0.2806105671514986</v>
       </c>
+      <c r="F79">
+        <v>0.3366336633663367</v>
+      </c>
     </row>
     <row r="80">
       <c r="A80">
@@ -1726,6 +1965,9 @@
       <c r="E80">
         <v>-1.01145349650571</v>
       </c>
+      <c r="F80">
+        <v>0.3663366336633663</v>
+      </c>
     </row>
     <row r="81">
       <c r="A81">
@@ -1743,6 +1985,9 @@
       <c r="E81">
         <v>0.4873943288436651</v>
       </c>
+      <c r="F81">
+        <v>0.0891089108910891</v>
+      </c>
     </row>
     <row r="82">
       <c r="A82">
@@ -1760,6 +2005,9 @@
       <c r="E82">
         <v>0.1062814485949258</v>
       </c>
+      <c r="F82">
+        <v>0.5841584158415841</v>
+      </c>
     </row>
     <row r="83">
       <c r="A83">
@@ -1777,6 +2025,9 @@
       <c r="E83">
         <v>-1.4319324922999</v>
       </c>
+      <c r="F83">
+        <v>0.1782178217821782</v>
+      </c>
     </row>
     <row r="84">
       <c r="A84">
@@ -1794,6 +2045,9 @@
       <c r="E84">
         <v>-0.3935366869626525</v>
       </c>
+      <c r="F84">
+        <v>0.0891089108910891</v>
+      </c>
     </row>
     <row r="85">
       <c r="A85">
@@ -1811,6 +2065,9 @@
       <c r="E85">
         <v>-0.5606543929844239</v>
       </c>
+      <c r="F85">
+        <v>0.2079207920792079</v>
+      </c>
     </row>
     <row r="86">
       <c r="A86">
@@ -1828,6 +2085,9 @@
       <c r="E86">
         <v>0.599132085287976</v>
       </c>
+      <c r="F86">
+        <v>0.4554455445544555</v>
+      </c>
     </row>
     <row r="87">
       <c r="A87">
@@ -1845,6 +2105,9 @@
       <c r="E87">
         <v>0.8168330134196947</v>
       </c>
+      <c r="F87">
+        <v>0.5148514851485149</v>
+      </c>
     </row>
     <row r="88">
       <c r="A88">
@@ -1862,6 +2125,9 @@
       <c r="E88">
         <v>0.6628614318802564</v>
       </c>
+      <c r="F88">
+        <v>0.6534653465346535</v>
+      </c>
     </row>
     <row r="89">
       <c r="A89">
@@ -1879,6 +2145,9 @@
       <c r="E89">
         <v>0.4535174043014062</v>
       </c>
+      <c r="F89">
+        <v>0.7326732673267327</v>
+      </c>
     </row>
     <row r="90">
       <c r="A90">
@@ -1896,6 +2165,9 @@
       <c r="E90">
         <v>0.9752403467664936</v>
       </c>
+      <c r="F90">
+        <v>0.1089108910891089</v>
+      </c>
     </row>
     <row r="91">
       <c r="A91">
@@ -1913,6 +2185,9 @@
       <c r="E91">
         <v>0.5008652080405497</v>
       </c>
+      <c r="F91">
+        <v>0.7029702970297029</v>
+      </c>
     </row>
     <row r="92">
       <c r="A92">
@@ -1930,6 +2205,9 @@
       <c r="E92">
         <v>0.3437987718401465</v>
       </c>
+      <c r="F92">
+        <v>0.7029702970297029</v>
+      </c>
     </row>
     <row r="93">
       <c r="A93">
@@ -1947,6 +2225,9 @@
       <c r="E93">
         <v>0.8019969017794188</v>
       </c>
+      <c r="F93">
+        <v>0.6039603960396039</v>
+      </c>
     </row>
     <row r="94">
       <c r="A94">
@@ -1964,6 +2245,9 @@
       <c r="E94">
         <v>0.5329072581327825</v>
       </c>
+      <c r="F94">
+        <v>0.9603960396039604</v>
+      </c>
     </row>
     <row r="95">
       <c r="A95">
@@ -1981,6 +2265,9 @@
       <c r="E95">
         <v>0.6999368636630207</v>
       </c>
+      <c r="F95">
+        <v>0.0297029702970297</v>
+      </c>
     </row>
     <row r="96">
       <c r="A96">
@@ -1998,6 +2285,9 @@
       <c r="E96">
         <v>0.7243594684546144</v>
       </c>
+      <c r="F96">
+        <v>0.1287128712871287</v>
+      </c>
     </row>
     <row r="97">
       <c r="A97">
@@ -2015,6 +2305,9 @@
       <c r="E97">
         <v>-1.243283371806402</v>
       </c>
+      <c r="F97">
+        <v>0.3663366336633663</v>
+      </c>
     </row>
     <row r="98">
       <c r="A98">
@@ -2032,6 +2325,9 @@
       <c r="E98">
         <v>1.428364576074725</v>
       </c>
+      <c r="F98">
+        <v>0.4752475247524752</v>
+      </c>
     </row>
     <row r="99">
       <c r="A99">
@@ -2049,6 +2345,9 @@
       <c r="E99">
         <v>1.035280704208773</v>
       </c>
+      <c r="F99">
+        <v>0.8514851485148515</v>
+      </c>
     </row>
     <row r="100">
       <c r="A100">
@@ -2066,6 +2365,9 @@
       <c r="E100">
         <v>0.8113582936409649</v>
       </c>
+      <c r="F100">
+        <v>0.4554455445544555</v>
+      </c>
     </row>
     <row r="101">
       <c r="A101">
@@ -2083,6 +2385,9 @@
       <c r="E101">
         <v>-1.254595960466663</v>
       </c>
+      <c r="F101">
+        <v>0.04950495049504951</v>
+      </c>
     </row>
     <row r="102">
       <c r="A102">
@@ -2100,6 +2405,9 @@
       <c r="E102">
         <v>-0.5967500458501511</v>
       </c>
+      <c r="F102">
+        <v>0.297029702970297</v>
+      </c>
     </row>
     <row r="103">
       <c r="A103">
@@ -2117,6 +2425,9 @@
       <c r="E103">
         <v>-0.185212612112139</v>
       </c>
+      <c r="F103">
+        <v>0.3861386138613861</v>
+      </c>
     </row>
     <row r="104">
       <c r="A104">
@@ -2134,6 +2445,9 @@
       <c r="E104">
         <v>0.7911364215216693</v>
       </c>
+      <c r="F104">
+        <v>0.5841584158415841</v>
+      </c>
     </row>
     <row r="105">
       <c r="A105">
@@ -2151,6 +2465,9 @@
       <c r="E105">
         <v>0.5672121841717448</v>
       </c>
+      <c r="F105">
+        <v>0.06930693069306931</v>
+      </c>
     </row>
     <row r="106">
       <c r="A106">
@@ -2168,6 +2485,9 @@
       <c r="E106">
         <v>0.6414028294157301</v>
       </c>
+      <c r="F106">
+        <v>0.2772277227722773</v>
+      </c>
     </row>
     <row r="107">
       <c r="A107">
@@ -2185,6 +2505,9 @@
       <c r="E107">
         <v>1.283494465074454</v>
       </c>
+      <c r="F107">
+        <v>0.7425742574257426</v>
+      </c>
     </row>
     <row r="108">
       <c r="A108">
@@ -2202,6 +2525,9 @@
       <c r="E108">
         <v>1.57247574300851</v>
       </c>
+      <c r="F108">
+        <v>0.1386138613861386</v>
+      </c>
     </row>
     <row r="109">
       <c r="A109">
@@ -2219,6 +2545,9 @@
       <c r="E109">
         <v>-0.3133233984716673</v>
       </c>
+      <c r="F109">
+        <v>0.8118811881188119</v>
+      </c>
     </row>
     <row r="110">
       <c r="A110">
@@ -2236,6 +2565,9 @@
       <c r="E110">
         <v>-0.4215654379300802</v>
       </c>
+      <c r="F110">
+        <v>0.7722772277227723</v>
+      </c>
     </row>
     <row r="111">
       <c r="A111">
@@ -2253,6 +2585,9 @@
       <c r="E111">
         <v>-1.098574192408025</v>
       </c>
+      <c r="F111">
+        <v>0.900990099009901</v>
+      </c>
     </row>
     <row r="112">
       <c r="A112">
@@ -2270,6 +2605,9 @@
       <c r="E112">
         <v>0.2934470996200748</v>
       </c>
+      <c r="F112">
+        <v>0.4455445544554456</v>
+      </c>
     </row>
     <row r="113">
       <c r="A113">
@@ -2287,6 +2625,9 @@
       <c r="E113">
         <v>-0.5090756194441483</v>
       </c>
+      <c r="F113">
+        <v>0.495049504950495</v>
+      </c>
     </row>
     <row r="114">
       <c r="A114">
@@ -2304,6 +2645,9 @@
       <c r="E114">
         <v>-0.7216765873444991</v>
       </c>
+      <c r="F114">
+        <v>0.9603960396039604</v>
+      </c>
     </row>
     <row r="115">
       <c r="A115">
@@ -2321,6 +2665,9 @@
       <c r="E115">
         <v>-0.1779092918983252</v>
       </c>
+      <c r="F115">
+        <v>0.0396039603960396</v>
+      </c>
     </row>
     <row r="116">
       <c r="A116">
@@ -2338,6 +2685,9 @@
       <c r="E116">
         <v>-0.8456881648041868</v>
       </c>
+      <c r="F116">
+        <v>0.0396039603960396</v>
+      </c>
     </row>
     <row r="117">
       <c r="A117">
@@ -2355,6 +2705,9 @@
       <c r="E117">
         <v>-0.659241366953574</v>
       </c>
+      <c r="F117">
+        <v>0.3465346534653465</v>
+      </c>
     </row>
     <row r="118">
       <c r="A118">
@@ -2372,6 +2725,9 @@
       <c r="E118">
         <v>-0.5345713068577211</v>
       </c>
+      <c r="F118">
+        <v>0.0396039603960396</v>
+      </c>
     </row>
     <row r="119">
       <c r="A119">
@@ -2389,6 +2745,9 @@
       <c r="E119">
         <v>0.2949042332416791</v>
       </c>
+      <c r="F119">
+        <v>0.7326732673267327</v>
+      </c>
     </row>
     <row r="120">
       <c r="A120">
@@ -2406,6 +2765,9 @@
       <c r="E120">
         <v>1.496754687458018</v>
       </c>
+      <c r="F120">
+        <v>0.7425742574257426</v>
+      </c>
     </row>
     <row r="121">
       <c r="A121">
@@ -2423,6 +2785,9 @@
       <c r="E121">
         <v>-1.29227367969706</v>
       </c>
+      <c r="F121">
+        <v>0.6237623762376238</v>
+      </c>
     </row>
     <row r="122">
       <c r="A122">
@@ -2440,6 +2805,9 @@
       <c r="E122">
         <v>1.025073093919038</v>
       </c>
+      <c r="F122">
+        <v>0.3069306930693069</v>
+      </c>
     </row>
     <row r="123">
       <c r="A123">
@@ -2457,6 +2825,9 @@
       <c r="E123">
         <v>-0.6394956629198273</v>
       </c>
+      <c r="F123">
+        <v>0.6039603960396039</v>
+      </c>
     </row>
     <row r="124">
       <c r="A124">
@@ -2474,6 +2845,9 @@
       <c r="E124">
         <v>-1.221687052272558</v>
       </c>
+      <c r="F124">
+        <v>0.9702970297029703</v>
+      </c>
     </row>
     <row r="125">
       <c r="A125">
@@ -2491,6 +2865,9 @@
       <c r="E125">
         <v>-1.492273150606963</v>
       </c>
+      <c r="F125">
+        <v>0.3762376237623762</v>
+      </c>
     </row>
     <row r="126">
       <c r="A126">
@@ -2508,6 +2885,9 @@
       <c r="E126">
         <v>-0.6315291809188518</v>
       </c>
+      <c r="F126">
+        <v>0.3663366336633663</v>
+      </c>
     </row>
     <row r="127">
       <c r="A127">
@@ -2525,6 +2905,9 @@
       <c r="E127">
         <v>0.1946049103725923</v>
       </c>
+      <c r="F127">
+        <v>0.4752475247524752</v>
+      </c>
     </row>
     <row r="128">
       <c r="A128">
@@ -2542,6 +2925,9 @@
       <c r="E128">
         <v>0.5124985150129325</v>
       </c>
+      <c r="F128">
+        <v>0.8712871287128713</v>
+      </c>
     </row>
     <row r="129">
       <c r="A129">
@@ -2559,6 +2945,9 @@
       <c r="E129">
         <v>-1.166301821921634</v>
       </c>
+      <c r="F129">
+        <v>0.9207920792079208</v>
+      </c>
     </row>
     <row r="130">
       <c r="A130">
@@ -2576,6 +2965,9 @@
       <c r="E130">
         <v>-0.5192338511576784</v>
       </c>
+      <c r="F130">
+        <v>0.5148514851485149</v>
+      </c>
     </row>
     <row r="131">
       <c r="A131">
@@ -2593,6 +2985,9 @@
       <c r="E131">
         <v>1.481989469195548</v>
       </c>
+      <c r="F131">
+        <v>0.0594059405940594</v>
+      </c>
     </row>
     <row r="132">
       <c r="A132">
@@ -2610,6 +3005,9 @@
       <c r="E132">
         <v>0.8760769510414896</v>
       </c>
+      <c r="F132">
+        <v>0.7722772277227723</v>
+      </c>
     </row>
     <row r="133">
       <c r="A133">
@@ -2627,6 +3025,9 @@
       <c r="E133">
         <v>1.32973647065803</v>
       </c>
+      <c r="F133">
+        <v>0.8514851485148515</v>
+      </c>
     </row>
     <row r="134">
       <c r="A134">
@@ -2644,6 +3045,9 @@
       <c r="E134">
         <v>-0.7888295620080429</v>
       </c>
+      <c r="F134">
+        <v>0.1485148514851485</v>
+      </c>
     </row>
     <row r="135">
       <c r="A135">
@@ -2661,6 +3065,9 @@
       <c r="E135">
         <v>-1.054943007081313</v>
       </c>
+      <c r="F135">
+        <v>0.8811881188118812</v>
+      </c>
     </row>
     <row r="136">
       <c r="A136">
@@ -2678,6 +3085,9 @@
       <c r="E136">
         <v>-2.195791454934753</v>
       </c>
+      <c r="F136">
+        <v>0.1782178217821782</v>
+      </c>
     </row>
     <row r="137">
       <c r="A137">
@@ -2695,6 +3105,9 @@
       <c r="E137">
         <v>-0.8223704443661629</v>
       </c>
+      <c r="F137">
+        <v>0.8217821782178217</v>
+      </c>
     </row>
     <row r="138">
       <c r="A138">
@@ -2712,6 +3125,9 @@
       <c r="E138">
         <v>-0.9292170286387915</v>
       </c>
+      <c r="F138">
+        <v>0.2475247524752475</v>
+      </c>
     </row>
     <row r="139">
       <c r="A139">
@@ -2729,6 +3145,9 @@
       <c r="E139">
         <v>-1.185915659703711</v>
       </c>
+      <c r="F139">
+        <v>0.09900990099009901</v>
+      </c>
     </row>
     <row r="140">
       <c r="A140">
@@ -2746,6 +3165,9 @@
       <c r="E140">
         <v>0.2738012024588454</v>
       </c>
+      <c r="F140">
+        <v>0.1782178217821782</v>
+      </c>
     </row>
     <row r="141">
       <c r="A141">
@@ -2763,6 +3185,9 @@
       <c r="E141">
         <v>-0.1658149141767485</v>
       </c>
+      <c r="F141">
+        <v>0.1485148514851485</v>
+      </c>
     </row>
     <row r="142">
       <c r="A142">
@@ -2780,6 +3205,9 @@
       <c r="E142">
         <v>0.8833054148134493</v>
       </c>
+      <c r="F142">
+        <v>0.8118811881188119</v>
+      </c>
     </row>
     <row r="143">
       <c r="A143">
@@ -2797,6 +3225,9 @@
       <c r="E143">
         <v>-0.9776603177926705</v>
       </c>
+      <c r="F143">
+        <v>0.5445544554455446</v>
+      </c>
     </row>
     <row r="144">
       <c r="A144">
@@ -2814,6 +3245,9 @@
       <c r="E144">
         <v>1.164230437731049</v>
       </c>
+      <c r="F144">
+        <v>0.8217821782178217</v>
+      </c>
     </row>
     <row r="145">
       <c r="A145">
@@ -2831,6 +3265,9 @@
       <c r="E145">
         <v>-0.3874927521712806</v>
       </c>
+      <c r="F145">
+        <v>0.5643564356435643</v>
+      </c>
     </row>
     <row r="146">
       <c r="A146">
@@ -2848,6 +3285,9 @@
       <c r="E146">
         <v>-1.507343404962415</v>
       </c>
+      <c r="F146">
+        <v>0.6039603960396039</v>
+      </c>
     </row>
     <row r="147">
       <c r="A147">
@@ -2865,6 +3305,9 @@
       <c r="E147">
         <v>-0.9083614342563887</v>
       </c>
+      <c r="F147">
+        <v>0.06930693069306931</v>
+      </c>
     </row>
     <row r="148">
       <c r="A148">
@@ -2882,6 +3325,9 @@
       <c r="E148">
         <v>1.152457891846737</v>
       </c>
+      <c r="F148">
+        <v>0.1188118811881188</v>
+      </c>
     </row>
     <row r="149">
       <c r="A149">
@@ -2899,6 +3345,9 @@
       <c r="E149">
         <v>0.5535521609400448</v>
       </c>
+      <c r="F149">
+        <v>0.1188118811881188</v>
+      </c>
     </row>
     <row r="150">
       <c r="A150">
@@ -2916,6 +3365,9 @@
       <c r="E150">
         <v>-0.6215169520101719</v>
       </c>
+      <c r="F150">
+        <v>0.07920792079207921</v>
+      </c>
     </row>
     <row r="151">
       <c r="A151">
@@ -2933,6 +3385,9 @@
       <c r="E151">
         <v>0.6921738479068603</v>
       </c>
+      <c r="F151">
+        <v>0.2079207920792079</v>
+      </c>
     </row>
     <row r="152">
       <c r="A152">
@@ -2950,6 +3405,9 @@
       <c r="E152">
         <v>-0.8982146638111064</v>
       </c>
+      <c r="F152">
+        <v>0.2475247524752475</v>
+      </c>
     </row>
     <row r="153">
       <c r="A153">
@@ -2967,6 +3425,9 @@
       <c r="E153">
         <v>0.5940425501023986</v>
       </c>
+      <c r="F153">
+        <v>0.6336633663366337</v>
+      </c>
     </row>
     <row r="154">
       <c r="A154">
@@ -2984,6 +3445,9 @@
       <c r="E154">
         <v>0.818510493664523</v>
       </c>
+      <c r="F154">
+        <v>0.0891089108910891</v>
+      </c>
     </row>
     <row r="155">
       <c r="A155">
@@ -3001,6 +3465,9 @@
       <c r="E155">
         <v>-1.20199863510387</v>
       </c>
+      <c r="F155">
+        <v>0.2475247524752475</v>
+      </c>
     </row>
     <row r="156">
       <c r="A156">
@@ -3018,6 +3485,9 @@
       <c r="E156">
         <v>-0.3597605621870353</v>
       </c>
+      <c r="F156">
+        <v>0.2673267326732673</v>
+      </c>
     </row>
     <row r="157">
       <c r="A157">
@@ -3035,6 +3505,9 @@
       <c r="E157">
         <v>-0.5304339221574138</v>
       </c>
+      <c r="F157">
+        <v>0.6336633663366337</v>
+      </c>
     </row>
     <row r="158">
       <c r="A158">
@@ -3052,6 +3525,9 @@
       <c r="E158">
         <v>0.8024904240886304</v>
       </c>
+      <c r="F158">
+        <v>0.8217821782178217</v>
+      </c>
     </row>
     <row r="159">
       <c r="A159">
@@ -3069,6 +3545,9 @@
       <c r="E159">
         <v>0.701016091003999</v>
       </c>
+      <c r="F159">
+        <v>0.0297029702970297</v>
+      </c>
     </row>
     <row r="160">
       <c r="A160">
@@ -3086,6 +3565,9 @@
       <c r="E160">
         <v>0.3646676341119129</v>
       </c>
+      <c r="F160">
+        <v>0.6039603960396039</v>
+      </c>
     </row>
     <row r="161">
       <c r="A161">
@@ -3103,6 +3585,9 @@
       <c r="E161">
         <v>1.196421908987729</v>
       </c>
+      <c r="F161">
+        <v>0.7326732673267327</v>
+      </c>
     </row>
     <row r="162">
       <c r="A162">
@@ -3120,6 +3605,9 @@
       <c r="E162">
         <v>-1.904493828069514</v>
       </c>
+      <c r="F162">
+        <v>0.2772277227722773</v>
+      </c>
     </row>
     <row r="163">
       <c r="A163">
@@ -3137,6 +3625,9 @@
       <c r="E163">
         <v>0.4953710033848174</v>
       </c>
+      <c r="F163">
+        <v>0.5445544554455446</v>
+      </c>
     </row>
     <row r="164">
       <c r="A164">
@@ -3154,6 +3645,9 @@
       <c r="E164">
         <v>0.577284213626286</v>
       </c>
+      <c r="F164">
+        <v>0.6039603960396039</v>
+      </c>
     </row>
     <row r="165">
       <c r="A165">
@@ -3171,6 +3665,9 @@
       <c r="E165">
         <v>0.7448512354050755</v>
       </c>
+      <c r="F165">
+        <v>0.2574257425742574</v>
+      </c>
     </row>
     <row r="166">
       <c r="A166">
@@ -3188,6 +3685,9 @@
       <c r="E166">
         <v>-0.8828625339457079</v>
       </c>
+      <c r="F166">
+        <v>0.8613861386138614</v>
+      </c>
     </row>
     <row r="167">
       <c r="A167">
@@ -3205,6 +3705,9 @@
       <c r="E167">
         <v>0.6072233012256609</v>
       </c>
+      <c r="F167">
+        <v>0.2178217821782178</v>
+      </c>
     </row>
     <row r="168">
       <c r="A168">
@@ -3222,6 +3725,9 @@
       <c r="E168">
         <v>1.535693936726193</v>
       </c>
+      <c r="F168">
+        <v>0.8118811881188119</v>
+      </c>
     </row>
     <row r="169">
       <c r="A169">
@@ -3239,6 +3745,9 @@
       <c r="E169">
         <v>0.6502076466249447</v>
       </c>
+      <c r="F169">
+        <v>0.3564356435643564</v>
+      </c>
     </row>
     <row r="170">
       <c r="A170">
@@ -3256,6 +3765,9 @@
       <c r="E170">
         <v>-1.220300127205939</v>
       </c>
+      <c r="F170">
+        <v>0.801980198019802</v>
+      </c>
     </row>
     <row r="171">
       <c r="A171">
@@ -3273,6 +3785,9 @@
       <c r="E171">
         <v>-2.651786378830054</v>
       </c>
+      <c r="F171">
+        <v>0.7920792079207921</v>
+      </c>
     </row>
     <row r="172">
       <c r="A172">
@@ -3290,6 +3805,9 @@
       <c r="E172">
         <v>1.460187013624222</v>
       </c>
+      <c r="F172">
+        <v>0.4851485148514851</v>
+      </c>
     </row>
     <row r="173">
       <c r="A173">
@@ -3307,6 +3825,9 @@
       <c r="E173">
         <v>-0.4094452134828251</v>
       </c>
+      <c r="F173">
+        <v>0.3861386138613861</v>
+      </c>
     </row>
     <row r="174">
       <c r="A174">
@@ -3324,6 +3845,9 @@
       <c r="E174">
         <v>-1.044951195731442</v>
       </c>
+      <c r="F174">
+        <v>0.7128712871287128</v>
+      </c>
     </row>
     <row r="175">
       <c r="A175">
@@ -3341,6 +3865,9 @@
       <c r="E175">
         <v>-1.021199856999156</v>
       </c>
+      <c r="F175">
+        <v>0.2475247524752475</v>
+      </c>
     </row>
     <row r="176">
       <c r="A176">
@@ -3358,6 +3885,9 @@
       <c r="E176">
         <v>1.536710252461491</v>
       </c>
+      <c r="F176">
+        <v>0.2772277227722773</v>
+      </c>
     </row>
     <row r="177">
       <c r="A177">
@@ -3375,6 +3905,9 @@
       <c r="E177">
         <v>0.2674241323395345</v>
       </c>
+      <c r="F177">
+        <v>0.2871287128712871</v>
+      </c>
     </row>
     <row r="178">
       <c r="A178">
@@ -3392,6 +3925,9 @@
       <c r="E178">
         <v>0.9666397823291554</v>
       </c>
+      <c r="F178">
+        <v>0.009900990099009901</v>
+      </c>
     </row>
     <row r="179">
       <c r="A179">
@@ -3409,6 +3945,9 @@
       <c r="E179">
         <v>-0.5126367565142792</v>
       </c>
+      <c r="F179">
+        <v>0.5544554455445545</v>
+      </c>
     </row>
     <row r="180">
       <c r="A180">
@@ -3426,6 +3965,9 @@
       <c r="E180">
         <v>1.130804128804273</v>
       </c>
+      <c r="F180">
+        <v>0.8811881188118812</v>
+      </c>
     </row>
     <row r="181">
       <c r="A181">
@@ -3443,6 +3985,9 @@
       <c r="E181">
         <v>1.105775153833798</v>
       </c>
+      <c r="F181">
+        <v>0.297029702970297</v>
+      </c>
     </row>
     <row r="182">
       <c r="A182">
@@ -3460,6 +4005,9 @@
       <c r="E182">
         <v>1.665676111710483</v>
       </c>
+      <c r="F182">
+        <v>0.009900990099009901</v>
+      </c>
     </row>
     <row r="183">
       <c r="A183">
@@ -3477,6 +4025,9 @@
       <c r="E183">
         <v>0.8196420964281901</v>
       </c>
+      <c r="F183">
+        <v>0.4653465346534654</v>
+      </c>
     </row>
     <row r="184">
       <c r="A184">
@@ -3494,6 +4045,9 @@
       <c r="E184">
         <v>0.7283419375725669</v>
       </c>
+      <c r="F184">
+        <v>0.1386138613861386</v>
+      </c>
     </row>
     <row r="185">
       <c r="A185">
@@ -3511,6 +4065,9 @@
       <c r="E185">
         <v>-0.2758000700954776</v>
       </c>
+      <c r="F185">
+        <v>0.8712871287128713</v>
+      </c>
     </row>
     <row r="186">
       <c r="A186">
@@ -3528,6 +4085,9 @@
       <c r="E186">
         <v>0.5201578820319105</v>
       </c>
+      <c r="F186">
+        <v>0.1782178217821782</v>
+      </c>
     </row>
     <row r="187">
       <c r="A187">
@@ -3545,6 +4105,9 @@
       <c r="E187">
         <v>0.3135595286098555</v>
       </c>
+      <c r="F187">
+        <v>0.2574257425742574</v>
+      </c>
     </row>
     <row r="188">
       <c r="A188">
@@ -3562,6 +4125,9 @@
       <c r="E188">
         <v>0.7553799916277176</v>
       </c>
+      <c r="F188">
+        <v>0.7722772277227723</v>
+      </c>
     </row>
     <row r="189">
       <c r="A189">
@@ -3579,6 +4145,9 @@
       <c r="E189">
         <v>-0.6780909072187853</v>
       </c>
+      <c r="F189">
+        <v>0.405940594059406</v>
+      </c>
     </row>
     <row r="190">
       <c r="A190">
@@ -3596,6 +4165,9 @@
       <c r="E190">
         <v>-0.9554586811642252</v>
       </c>
+      <c r="F190">
+        <v>0.9603960396039604</v>
+      </c>
     </row>
     <row r="191">
       <c r="A191">
@@ -3613,6 +4185,9 @@
       <c r="E191">
         <v>-1.204844244229299</v>
       </c>
+      <c r="F191">
+        <v>0.7128712871287128</v>
+      </c>
     </row>
     <row r="192">
       <c r="A192">
@@ -3630,6 +4205,9 @@
       <c r="E192">
         <v>-1.016089289667355</v>
       </c>
+      <c r="F192">
+        <v>0.8712871287128713</v>
+      </c>
     </row>
     <row r="193">
       <c r="A193">
@@ -3647,6 +4225,9 @@
       <c r="E193">
         <v>-0.9835364686611751</v>
       </c>
+      <c r="F193">
+        <v>0.8514851485148515</v>
+      </c>
     </row>
     <row r="194">
       <c r="A194">
@@ -3664,6 +4245,9 @@
       <c r="E194">
         <v>-0.9904452818093369</v>
       </c>
+      <c r="F194">
+        <v>0.6633663366336634</v>
+      </c>
     </row>
     <row r="195">
       <c r="A195">
@@ -3681,6 +4265,9 @@
       <c r="E195">
         <v>-0.6743163628198936</v>
       </c>
+      <c r="F195">
+        <v>0.7623762376237624</v>
+      </c>
     </row>
     <row r="196">
       <c r="A196">
@@ -3698,6 +4285,9 @@
       <c r="E196">
         <v>-0.2582755890451793</v>
       </c>
+      <c r="F196">
+        <v>0.3663366336633663</v>
+      </c>
     </row>
     <row r="197">
       <c r="A197">
@@ -3715,6 +4305,9 @@
       <c r="E197">
         <v>0.9545077189862916</v>
       </c>
+      <c r="F197">
+        <v>0.6336633663366337</v>
+      </c>
     </row>
     <row r="198">
       <c r="A198">
@@ -3732,6 +4325,9 @@
       <c r="E198">
         <v>-0.8703383700463511</v>
       </c>
+      <c r="F198">
+        <v>0.0297029702970297</v>
+      </c>
     </row>
     <row r="199">
       <c r="A199">
@@ -3749,6 +4345,9 @@
       <c r="E199">
         <v>-0.8636608908773576</v>
       </c>
+      <c r="F199">
+        <v>0.7425742574257426</v>
+      </c>
     </row>
     <row r="200">
       <c r="A200">
@@ -3766,6 +4365,9 @@
       <c r="E200">
         <v>-1.087437911459352</v>
       </c>
+      <c r="F200">
+        <v>0.3564356435643564</v>
+      </c>
     </row>
     <row r="201">
       <c r="A201">
@@ -3783,6 +4385,9 @@
       <c r="E201">
         <v>-0.7823956860095156</v>
       </c>
+      <c r="F201">
+        <v>0.06930693069306931</v>
+      </c>
     </row>
     <row r="202">
       <c r="A202">
@@ -3800,6 +4405,9 @@
       <c r="E202">
         <v>-0.8312087675674783</v>
       </c>
+      <c r="F202">
+        <v>0.405940594059406</v>
+      </c>
     </row>
     <row r="203">
       <c r="A203">
@@ -3817,6 +4425,9 @@
       <c r="E203">
         <v>0.276275429511213</v>
       </c>
+      <c r="F203">
+        <v>0.1485148514851485</v>
+      </c>
     </row>
     <row r="204">
       <c r="A204">
@@ -3834,6 +4445,9 @@
       <c r="E204">
         <v>1.023570228270207</v>
       </c>
+      <c r="F204">
+        <v>0.7821782178217822</v>
+      </c>
     </row>
     <row r="205">
       <c r="A205">
@@ -3851,6 +4465,9 @@
       <c r="E205">
         <v>0.4652972975520023</v>
       </c>
+      <c r="F205">
+        <v>0.6138613861386139</v>
+      </c>
     </row>
     <row r="206">
       <c r="A206">
@@ -3868,6 +4485,9 @@
       <c r="E206">
         <v>-0.9828853086554971</v>
       </c>
+      <c r="F206">
+        <v>0.900990099009901</v>
+      </c>
     </row>
     <row r="207">
       <c r="A207">
@@ -3885,6 +4505,9 @@
       <c r="E207">
         <v>1.213451406058078</v>
       </c>
+      <c r="F207">
+        <v>0.6831683168316832</v>
+      </c>
     </row>
     <row r="208">
       <c r="A208">
@@ -3902,6 +4525,9 @@
       <c r="E208">
         <v>0.1752902639356047</v>
       </c>
+      <c r="F208">
+        <v>0.0198019801980198</v>
+      </c>
     </row>
     <row r="209">
       <c r="A209">
@@ -3919,6 +4545,9 @@
       <c r="E209">
         <v>0.2383542887239849</v>
       </c>
+      <c r="F209">
+        <v>0.5643564356435643</v>
+      </c>
     </row>
     <row r="210">
       <c r="A210">
@@ -3936,6 +4565,9 @@
       <c r="E210">
         <v>0.7064435014840748</v>
       </c>
+      <c r="F210">
+        <v>0.2673267326732673</v>
+      </c>
     </row>
     <row r="211">
       <c r="A211">
@@ -3953,6 +4585,9 @@
       <c r="E211">
         <v>0.47525268120346</v>
       </c>
+      <c r="F211">
+        <v>0.9801980198019802</v>
+      </c>
     </row>
     <row r="212">
       <c r="A212">
@@ -3970,6 +4605,9 @@
       <c r="E212">
         <v>1.269675542545683</v>
       </c>
+      <c r="F212">
+        <v>0.5445544554455446</v>
+      </c>
     </row>
     <row r="213">
       <c r="A213">
@@ -3987,6 +4625,9 @@
       <c r="E213">
         <v>1.257012908685231</v>
       </c>
+      <c r="F213">
+        <v>0.9306930693069307</v>
+      </c>
     </row>
     <row r="214">
       <c r="A214">
@@ -4004,6 +4645,9 @@
       <c r="E214">
         <v>-0.9315413015086903</v>
       </c>
+      <c r="F214">
+        <v>0.1089108910891089</v>
+      </c>
     </row>
     <row r="215">
       <c r="A215">
@@ -4021,6 +4665,9 @@
       <c r="E215">
         <v>-0.7110100081708212</v>
       </c>
+      <c r="F215">
+        <v>0.9306930693069307</v>
+      </c>
     </row>
     <row r="216">
       <c r="A216">
@@ -4038,6 +4685,9 @@
       <c r="E216">
         <v>1.309966883994103</v>
       </c>
+      <c r="F216">
+        <v>0.297029702970297</v>
+      </c>
     </row>
     <row r="217">
       <c r="A217">
@@ -4055,6 +4705,9 @@
       <c r="E217">
         <v>-1.056724679267986</v>
       </c>
+      <c r="F217">
+        <v>0.5247524752475248</v>
+      </c>
     </row>
     <row r="218">
       <c r="A218">
@@ -4072,6 +4725,9 @@
       <c r="E218">
         <v>-0.5674488776562985</v>
       </c>
+      <c r="F218">
+        <v>0.7425742574257426</v>
+      </c>
     </row>
     <row r="219">
       <c r="A219">
@@ -4089,6 +4745,9 @@
       <c r="E219">
         <v>-0.692176641929674</v>
       </c>
+      <c r="F219">
+        <v>0.1881188118811881</v>
+      </c>
     </row>
     <row r="220">
       <c r="A220">
@@ -4106,6 +4765,9 @@
       <c r="E220">
         <v>-1.237052703802109</v>
       </c>
+      <c r="F220">
+        <v>0.4851485148514851</v>
+      </c>
     </row>
     <row r="221">
       <c r="A221">
@@ -4123,6 +4785,9 @@
       <c r="E221">
         <v>0.4202294666445029</v>
       </c>
+      <c r="F221">
+        <v>0.9801980198019802</v>
+      </c>
     </row>
     <row r="222">
       <c r="A222">
@@ -4140,6 +4805,9 @@
       <c r="E222">
         <v>0.1125545089794923</v>
       </c>
+      <c r="F222">
+        <v>0.5544554455445545</v>
+      </c>
     </row>
     <row r="223">
       <c r="A223">
@@ -4157,6 +4825,9 @@
       <c r="E223">
         <v>0.3931264024427058</v>
       </c>
+      <c r="F223">
+        <v>0.3267326732673267</v>
+      </c>
     </row>
     <row r="224">
       <c r="A224">
@@ -4174,6 +4845,9 @@
       <c r="E224">
         <v>-1.242984540431493</v>
       </c>
+      <c r="F224">
+        <v>0.7227722772277227</v>
+      </c>
     </row>
     <row r="225">
       <c r="A225">
@@ -4191,6 +4865,9 @@
       <c r="E225">
         <v>-0.3685835866858503</v>
       </c>
+      <c r="F225">
+        <v>0.5445544554455446</v>
+      </c>
     </row>
     <row r="226">
       <c r="A226">
@@ -4208,6 +4885,9 @@
       <c r="E226">
         <v>-0.8565666726934653</v>
       </c>
+      <c r="F226">
+        <v>0.5247524752475248</v>
+      </c>
     </row>
     <row r="227">
       <c r="A227">
@@ -4225,6 +4905,9 @@
       <c r="E227">
         <v>-0.3631803869652636</v>
       </c>
+      <c r="F227">
+        <v>0.9108910891089109</v>
+      </c>
     </row>
     <row r="228">
       <c r="A228">
@@ -4242,6 +4925,9 @@
       <c r="E228">
         <v>-2.038504021890902</v>
       </c>
+      <c r="F228">
+        <v>0.5346534653465347</v>
+      </c>
     </row>
     <row r="229">
       <c r="A229">
@@ -4259,6 +4945,9 @@
       <c r="E229">
         <v>-0.3621565169313372</v>
       </c>
+      <c r="F229">
+        <v>0.297029702970297</v>
+      </c>
     </row>
     <row r="230">
       <c r="A230">
@@ -4276,6 +4965,9 @@
       <c r="E230">
         <v>-0.3959962503786589</v>
       </c>
+      <c r="F230">
+        <v>0.594059405940594</v>
+      </c>
     </row>
     <row r="231">
       <c r="A231">
@@ -4293,6 +4985,9 @@
       <c r="E231">
         <v>-0.7389322512537744</v>
       </c>
+      <c r="F231">
+        <v>0.6435643564356436</v>
+      </c>
     </row>
     <row r="232">
       <c r="A232">
@@ -4310,6 +5005,9 @@
       <c r="E232">
         <v>0.235526717053235</v>
       </c>
+      <c r="F232">
+        <v>0.5841584158415841</v>
+      </c>
     </row>
     <row r="233">
       <c r="A233">
@@ -4327,6 +5025,9 @@
       <c r="E233">
         <v>-0.1398114571441243</v>
       </c>
+      <c r="F233">
+        <v>0.2772277227722773</v>
+      </c>
     </row>
     <row r="234">
       <c r="A234">
@@ -4344,6 +5045,9 @@
       <c r="E234">
         <v>-0.6130550774633811</v>
       </c>
+      <c r="F234">
+        <v>0.9504950495049505</v>
+      </c>
     </row>
     <row r="235">
       <c r="A235">
@@ -4361,6 +5065,9 @@
       <c r="E235">
         <v>-1.784671671020122</v>
       </c>
+      <c r="F235">
+        <v>0.2673267326732673</v>
+      </c>
     </row>
     <row r="236">
       <c r="A236">
@@ -4378,6 +5085,9 @@
       <c r="E236">
         <v>0.5042325823406385</v>
       </c>
+      <c r="F236">
+        <v>0.6633663366336634</v>
+      </c>
     </row>
     <row r="237">
       <c r="A237">
@@ -4395,6 +5105,9 @@
       <c r="E237">
         <v>0.821520476094962</v>
       </c>
+      <c r="F237">
+        <v>0.0396039603960396</v>
+      </c>
     </row>
     <row r="238">
       <c r="A238">
@@ -4412,6 +5125,9 @@
       <c r="E238">
         <v>1.178821564312267</v>
       </c>
+      <c r="F238">
+        <v>0.2277227722772277</v>
+      </c>
     </row>
     <row r="239">
       <c r="A239">
@@ -4429,6 +5145,9 @@
       <c r="E239">
         <v>-0.4264357868748339</v>
       </c>
+      <c r="F239">
+        <v>0.1188118811881188</v>
+      </c>
     </row>
     <row r="240">
       <c r="A240">
@@ -4446,6 +5165,9 @@
       <c r="E240">
         <v>0.8652913243194275</v>
       </c>
+      <c r="F240">
+        <v>0.7326732673267327</v>
+      </c>
     </row>
     <row r="241">
       <c r="A241">
@@ -4463,6 +5185,9 @@
       <c r="E241">
         <v>0.4681870817846309</v>
       </c>
+      <c r="F241">
+        <v>0.4158415841584158</v>
+      </c>
     </row>
     <row r="242">
       <c r="A242">
@@ -4480,6 +5205,9 @@
       <c r="E242">
         <v>-0.4680454816535866</v>
       </c>
+      <c r="F242">
+        <v>0.07920792079207921</v>
+      </c>
     </row>
     <row r="243">
       <c r="A243">
@@ -4497,6 +5225,9 @@
       <c r="E243">
         <v>-0.4604370680297061</v>
       </c>
+      <c r="F243">
+        <v>0.1584158415841584</v>
+      </c>
     </row>
     <row r="244">
       <c r="A244">
@@ -4514,6 +5245,9 @@
       <c r="E244">
         <v>0.879779577730823</v>
       </c>
+      <c r="F244">
+        <v>0.5247524752475248</v>
+      </c>
     </row>
     <row r="245">
       <c r="A245">
@@ -4531,6 +5265,9 @@
       <c r="E245">
         <v>-0.9273251217333616</v>
       </c>
+      <c r="F245">
+        <v>0.06930693069306931</v>
+      </c>
     </row>
     <row r="246">
       <c r="A246">
@@ -4548,6 +5285,9 @@
       <c r="E246">
         <v>-0.9836062666997404</v>
       </c>
+      <c r="F246">
+        <v>0.3564356435643564</v>
+      </c>
     </row>
     <row r="247">
       <c r="A247">
@@ -4565,6 +5305,9 @@
       <c r="E247">
         <v>-2.070176240112521</v>
       </c>
+      <c r="F247">
+        <v>0.7326732673267327</v>
+      </c>
     </row>
     <row r="248">
       <c r="A248">
@@ -4582,6 +5325,9 @@
       <c r="E248">
         <v>0.6702100701163815</v>
       </c>
+      <c r="F248">
+        <v>0.4356435643564356</v>
+      </c>
     </row>
     <row r="249">
       <c r="A249">
@@ -4599,6 +5345,9 @@
       <c r="E249">
         <v>0.9082593881409999</v>
       </c>
+      <c r="F249">
+        <v>0.7326732673267327</v>
+      </c>
     </row>
     <row r="250">
       <c r="A250">
@@ -4616,6 +5365,9 @@
       <c r="E250">
         <v>0.0508429998103552</v>
       </c>
+      <c r="F250">
+        <v>0.5445544554455446</v>
+      </c>
     </row>
     <row r="251">
       <c r="A251">
@@ -4632,6 +5384,9 @@
       </c>
       <c r="E251">
         <v>0.6692839125030677</v>
+      </c>
+      <c r="F251">
+        <v>0.07920792079207921</v>
       </c>
     </row>
   </sheetData>

</xml_diff>